<commit_message>
Ronda 2 hoy 14/06
</commit_message>
<xml_diff>
--- a/Rancho/asignaciones.xlsx
+++ b/Rancho/asignaciones.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="54">
   <si>
     <t>Movil</t>
   </si>
@@ -25,136 +25,139 @@
     <t>Imagen</t>
   </si>
   <si>
-    <t>52_7757554731</t>
-  </si>
-  <si>
-    <t>52_7757573183</t>
-  </si>
-  <si>
-    <t>52_7757582047</t>
-  </si>
-  <si>
-    <t>52_7757605307</t>
-  </si>
-  <si>
-    <t>52_7757847752</t>
-  </si>
-  <si>
-    <t>52_7761061274</t>
-  </si>
-  <si>
-    <t>52_7751144050</t>
-  </si>
-  <si>
-    <t>52_7752349890</t>
-  </si>
-  <si>
-    <t>52_7752250115</t>
-  </si>
-  <si>
-    <t>52_7711916618</t>
-  </si>
-  <si>
-    <t>52_7752142659</t>
-  </si>
-  <si>
-    <t>52_5512577630</t>
-  </si>
-  <si>
-    <t>52_5514836649</t>
-  </si>
-  <si>
-    <t>52_5574913650</t>
-  </si>
-  <si>
-    <t>52_5582872819</t>
-  </si>
-  <si>
-    <t>52_5585795791</t>
-  </si>
-  <si>
-    <t>52_7712142411</t>
-  </si>
-  <si>
-    <t>52_7716832240</t>
-  </si>
-  <si>
-    <t>52_7717002536</t>
-  </si>
-  <si>
-    <t>52_7717515336</t>
-  </si>
-  <si>
-    <t>52_7751018598</t>
-  </si>
-  <si>
-    <t>52_7751042979</t>
-  </si>
-  <si>
-    <t>52_7751156262</t>
-  </si>
-  <si>
-    <t>52_7751183348</t>
-  </si>
-  <si>
-    <t>52_7714402628</t>
-  </si>
-  <si>
-    <t>52_7751194697</t>
-  </si>
-  <si>
-    <t>52_7751196618</t>
-  </si>
-  <si>
-    <t>52_7751222770</t>
-  </si>
-  <si>
-    <t>52_7751253082</t>
-  </si>
-  <si>
-    <t>52_7751273964</t>
-  </si>
-  <si>
-    <t>52_7751342273</t>
-  </si>
-  <si>
-    <t>52_7751291667</t>
-  </si>
-  <si>
-    <t>52_7751191720</t>
-  </si>
-  <si>
-    <t>52_7751345491</t>
-  </si>
-  <si>
-    <t>52_7751362982</t>
-  </si>
-  <si>
-    <t>52_7751366634</t>
-  </si>
-  <si>
-    <t>52_7751384498</t>
-  </si>
-  <si>
-    <t>52_7751393720</t>
-  </si>
-  <si>
-    <t>52_7751428201</t>
-  </si>
-  <si>
-    <t>52_7751431775</t>
-  </si>
-  <si>
-    <t>52_7751434290</t>
-  </si>
-  <si>
-    <t>52_7751452644</t>
-  </si>
-  <si>
-    <t>52_7751484017</t>
-  </si>
-  <si>
-    <t>52_7751493612</t>
+    <t>52_7751441859</t>
+  </si>
+  <si>
+    <t>52_7751456754</t>
+  </si>
+  <si>
+    <t>52_7751537112</t>
+  </si>
+  <si>
+    <t>52_7751551945</t>
+  </si>
+  <si>
+    <t>52_7751605551</t>
+  </si>
+  <si>
+    <t>52_7751609397</t>
+  </si>
+  <si>
+    <t>52_7751618134</t>
+  </si>
+  <si>
+    <t>52_7751674759</t>
+  </si>
+  <si>
+    <t>52_7751820501</t>
+  </si>
+  <si>
+    <t>52_7751855523</t>
+  </si>
+  <si>
+    <t>52_7751916237</t>
+  </si>
+  <si>
+    <t>52_7751928351</t>
+  </si>
+  <si>
+    <t>52_7751937397</t>
+  </si>
+  <si>
+    <t>52_7751980213</t>
+  </si>
+  <si>
+    <t>52_7751995043</t>
+  </si>
+  <si>
+    <t>52_7752018495</t>
+  </si>
+  <si>
+    <t>52_7752018993</t>
+  </si>
+  <si>
+    <t>52_7752026064</t>
+  </si>
+  <si>
+    <t>52_7752054219</t>
+  </si>
+  <si>
+    <t>52_7752055804</t>
+  </si>
+  <si>
+    <t>52_7752055827</t>
+  </si>
+  <si>
+    <t>52_7752061930</t>
+  </si>
+  <si>
+    <t>52_7752212730</t>
+  </si>
+  <si>
+    <t>52_7752282291</t>
+  </si>
+  <si>
+    <t>52_7752356335</t>
+  </si>
+  <si>
+    <t>52_7752359588</t>
+  </si>
+  <si>
+    <t>52_7752361643</t>
+  </si>
+  <si>
+    <t>52_7752509898</t>
+  </si>
+  <si>
+    <t>52_7752534040</t>
+  </si>
+  <si>
+    <t>52_7757067426</t>
+  </si>
+  <si>
+    <t>52_7751458051</t>
+  </si>
+  <si>
+    <t>52_7751357889</t>
+  </si>
+  <si>
+    <t>52_7757548955</t>
+  </si>
+  <si>
+    <t>52_5579934304</t>
+  </si>
+  <si>
+    <t>52_7751056494</t>
+  </si>
+  <si>
+    <t>52_7751323350</t>
+  </si>
+  <si>
+    <t>52_7751373509</t>
+  </si>
+  <si>
+    <t>52_7712029807</t>
+  </si>
+  <si>
+    <t>52_7712059478</t>
+  </si>
+  <si>
+    <t>52_7751036577</t>
+  </si>
+  <si>
+    <t>52_7751244729</t>
+  </si>
+  <si>
+    <t>52_7751267907</t>
+  </si>
+  <si>
+    <t>52_7751279804</t>
+  </si>
+  <si>
+    <t>52_7751280849</t>
+  </si>
+  <si>
+    <t>52_7751315193</t>
   </si>
   <si>
     <t>📢Le presento la Privada *★Olivo, Modelo Lugo★*
@@ -590,7 +593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -612,10 +615,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -623,10 +626,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -634,10 +637,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -645,10 +648,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -656,10 +659,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -667,10 +670,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -678,10 +681,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -689,10 +692,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -700,10 +703,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -711,10 +714,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -722,10 +725,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -733,10 +736,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -744,10 +747,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -755,10 +758,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -766,10 +769,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -777,10 +780,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -788,10 +791,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -799,10 +802,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -810,10 +813,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -821,10 +824,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -832,10 +835,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -843,10 +846,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -854,10 +857,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -865,10 +868,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -876,10 +879,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -887,10 +890,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -898,10 +901,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -909,10 +912,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -920,10 +923,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -931,10 +934,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -942,10 +945,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -953,10 +956,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -964,10 +967,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -975,10 +978,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -986,10 +989,10 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -997,10 +1000,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1008,10 +1011,10 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1019,10 +1022,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1030,10 +1033,10 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1041,10 +1044,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1052,10 +1055,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1063,10 +1066,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1074,10 +1077,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1085,9 +1088,20 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>